<commit_message>
Microcontroller schematic sheet with decoupling, crystals, RF matching etc. Various app notes
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0dc02c4a829257e4/Documents/Personal/projects/bluetooth-audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="299" documentId="8_{4FB5AB32-D425-4BE6-BD36-2E3FAA4B4BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C451206C-ED10-4C64-BA6E-9FDEF17C9352}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="8_{4FB5AB32-D425-4BE6-BD36-2E3FAA4B4BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DFCDB8C-915D-4E92-BBF4-972EF1D658AA}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{49D08A49-7D4D-4255-9C0B-B147CF678ED3}"/>
+    <workbookView minimized="1" xWindow="19155" yWindow="-16200" windowWidth="16080" windowHeight="9255" activeTab="1" xr2:uid="{49D08A49-7D4D-4255-9C0B-B147CF678ED3}"/>
   </bookViews>
   <sheets>
     <sheet name="Buck converter" sheetId="1" r:id="rId1"/>
+    <sheet name="RF" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -257,7 +258,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;R&quot;#,##0;[Red]\-&quot;R&quot;#,##0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -338,20 +339,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -685,6 +685,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>311727</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>52304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{618C1D49-BE40-7C7F-10CB-B104C586F123}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="640773" y="346365"/>
+          <a:ext cx="5437909" cy="4555030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1004,7 +1053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E0CDA7-FFA5-4B65-AC33-99D61553F876}">
   <dimension ref="A20:Y97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R49" sqref="R49"/>
     </sheetView>
   </sheetViews>
@@ -1047,7 +1096,7 @@
       <c r="Q37" t="s">
         <v>19</v>
       </c>
-      <c r="R37" s="10" t="s">
+      <c r="R37" t="s">
         <v>70</v>
       </c>
       <c r="S37" s="1" t="s">
@@ -1442,4 +1491,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBA4D58-95DE-4AC6-A317-818729DB4475}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Custom symbol and footprints for IS2083. Updated design document. Initial dump of components onto cleared PCB.
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0dc02c4a829257e4/Documents/Personal/projects/bluetooth-audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="826" documentId="8_{4FB5AB32-D425-4BE6-BD36-2E3FAA4B4BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C4D5E3-1B8E-43B9-8994-F3424C718E1A}"/>
+  <xr:revisionPtr revIDLastSave="1018" documentId="8_{4FB5AB32-D425-4BE6-BD36-2E3FAA4B4BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D6CCCD7-12E2-41DC-B723-D8EBBDFEA58E}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{49D08A49-7D4D-4255-9C0B-B147CF678ED3}"/>
   </bookViews>
@@ -16,9 +16,12 @@
     <sheet name="System design" sheetId="3" r:id="rId1"/>
     <sheet name="ESP-32" sheetId="4" r:id="rId2"/>
     <sheet name="Specifications" sheetId="5" r:id="rId3"/>
-    <sheet name="PCB checks" sheetId="6" r:id="rId4"/>
-    <sheet name="Power" sheetId="1" r:id="rId5"/>
-    <sheet name="STM32WB" sheetId="2" r:id="rId6"/>
+    <sheet name="IS2083" sheetId="9" r:id="rId4"/>
+    <sheet name="STM32F4 + CC2564" sheetId="7" r:id="rId5"/>
+    <sheet name="Power budget" sheetId="8" r:id="rId6"/>
+    <sheet name="PCB checks" sheetId="6" r:id="rId7"/>
+    <sheet name="Power" sheetId="1" r:id="rId8"/>
+    <sheet name="STM32WB" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="354">
   <si>
     <t>Ilp-p</t>
   </si>
@@ -910,6 +913,206 @@
   </si>
   <si>
     <t>Check USB footprint</t>
+  </si>
+  <si>
+    <t>STM32 VCC = 3v3</t>
+  </si>
+  <si>
+    <t>CC2564 VCC = 1v8</t>
+  </si>
+  <si>
+    <t>Rechargeable via USB-C PD</t>
+  </si>
+  <si>
+    <t>Current sufficient to power Micro, codec, bluetooth controller</t>
+  </si>
+  <si>
+    <t>STM32 DAC not perfect for audio - use separate stereo codec</t>
+  </si>
+  <si>
+    <t>uC - ES8388 interface - i2c for configuration</t>
+  </si>
+  <si>
+    <t>BT controller - ES interface: i2s bypasses uC</t>
+  </si>
+  <si>
+    <t>Full duplex audio required for ES8388 to BTC over i2s</t>
+  </si>
+  <si>
+    <t>ES8388 connects to barrel jack on one of the line out channels</t>
+  </si>
+  <si>
+    <t>Bluetooth controller + uC</t>
+  </si>
+  <si>
+    <t>TI CC2564 dual mode BT controller (HCI) - host controlled interface - requires separate uC</t>
+  </si>
+  <si>
+    <t>TI CC2564</t>
+  </si>
+  <si>
+    <t>STM32F4 has built in flash</t>
+  </si>
+  <si>
+    <t>Option to reset the uC</t>
+  </si>
+  <si>
+    <t>Check reset connection / flow to BTC</t>
+  </si>
+  <si>
+    <t>External MHz crystal required for STM32</t>
+  </si>
+  <si>
+    <t>Spec crystal load caps as per ST app note</t>
+  </si>
+  <si>
+    <t>Visual indicators for uC</t>
+  </si>
+  <si>
+    <t>STM32F4 has built in USB controller. But also include SWD</t>
+  </si>
+  <si>
+    <t>Confirm for STM</t>
+  </si>
+  <si>
+    <t>SWD, and JTAG debugging can be broken out separately</t>
+  </si>
+  <si>
+    <t>Powered from lithium coin cell</t>
+  </si>
+  <si>
+    <t>Vin = 3.2 - 4.2V (3.7V nominal)</t>
+  </si>
+  <si>
+    <t>TPS63802DLAR (0.6USD)</t>
+  </si>
+  <si>
+    <t>MCP73831</t>
+  </si>
+  <si>
+    <t>Battery that can supply 100mA</t>
+  </si>
+  <si>
+    <t>LIR2450</t>
+  </si>
+  <si>
+    <t>battery holder</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Keystone-3008TR/C238100</t>
+  </si>
+  <si>
+    <t>STM32F4</t>
+  </si>
+  <si>
+    <t>CC2564</t>
+  </si>
+  <si>
+    <t>Working V</t>
+  </si>
+  <si>
+    <t>Power (mW)</t>
+  </si>
+  <si>
+    <t>112mA</t>
+  </si>
+  <si>
+    <t>Current (mA)</t>
+  </si>
+  <si>
+    <t>STM32 + CC2564 based system</t>
+  </si>
+  <si>
+    <t>IS2083 all in one SoC system</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>Receiver</t>
+  </si>
+  <si>
+    <t>A2DP mode</t>
+  </si>
+  <si>
+    <t>Continuous RX</t>
+  </si>
+  <si>
+    <t>Continuous TX</t>
+  </si>
+  <si>
+    <t>Built in Li-ion / LiPo charger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS2083 A2DP: 12mA
+Continuous TX/RX: Max 50mA
+DAC: 8mA
+</t>
+  </si>
+  <si>
+    <t>LIR2450 - coin cell, max 125 mA, 120mAh</t>
+  </si>
+  <si>
+    <t>SMD, fits LIR2450, bottom side mounted</t>
+  </si>
+  <si>
+    <t>Support MIC in, stereo audio out</t>
+  </si>
+  <si>
+    <t>IS2083 has built in DAC / Codec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS2083 supports single stereo digital MIC or dual analog stereo.
+</t>
+  </si>
+  <si>
+    <t>(Optional) - audio in via AUX</t>
+  </si>
+  <si>
+    <t>Configure uC as Audio Transceiver</t>
+  </si>
+  <si>
+    <t>Dual Mode Bluetooth SoC</t>
+  </si>
+  <si>
+    <t>IS2083BM implements A2DP sink, HFP</t>
+  </si>
+  <si>
+    <t>LIR2450 - CC 24mA CV 4.20V
+IS2083 accepts 5V (ADAP_IN) to charge battery - wire this from USB-C</t>
+  </si>
+  <si>
+    <t>External MHz crystal required for uC</t>
+  </si>
+  <si>
+    <t>16MHz with external load caps</t>
+  </si>
+  <si>
+    <t>2x LEDS, Blue, green, connect to IS2083 LED driver (can sink 0.35mA each)</t>
+  </si>
+  <si>
+    <t>Yes, external HW reset, active low (RST_N)</t>
+  </si>
+  <si>
+    <t>IS2083BM has built in flash (16MBit / 2MB)</t>
+  </si>
+  <si>
+    <t>2 wire JTAG built in</t>
+  </si>
+  <si>
+    <t>Control buttons</t>
+  </si>
+  <si>
+    <t>GPIO pins available for FWD, PLAY/PAUSE, REV, VOL_DB, VOL_UP</t>
+  </si>
+  <si>
+    <t>uC, codec, bluetooth transceiver all in one</t>
+  </si>
+  <si>
+    <t>Use IS2083BM in embedded mode</t>
+  </si>
+  <si>
+    <t>Matching PI network required (specified in Datasheet)</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1263,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1109,6 +1312,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1117,6 +1338,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2508,7 +2732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F18407-E529-4114-A56B-CDB1C2979C9E}">
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2583,8 +2807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFFBAFF-8947-4084-92DD-D93B3A44A18A}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2598,15 +2822,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
@@ -2938,15 +3162,15 @@
     </row>
     <row r="25" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="26" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="25"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
@@ -3606,11 +3830,1707 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A56080-762C-4044-85B6-92A46EF95B07}">
+  <dimension ref="A1:G81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.796875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="61.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.265625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="12"/>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="12"/>
+      <c r="B3" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="12"/>
+      <c r="B5" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="E5" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A6" s="12"/>
+      <c r="B6" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="12"/>
+      <c r="B7" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="12"/>
+      <c r="B8" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C8" t="s">
+        <v>334</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="E8" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="12"/>
+      <c r="E9" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="12"/>
+      <c r="E10" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="12"/>
+      <c r="E11" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="12"/>
+      <c r="E12" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="12"/>
+      <c r="B13" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" t="s">
+        <v>335</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="E14" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="12"/>
+      <c r="E15" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="12"/>
+      <c r="E16" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E17" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="12"/>
+      <c r="B18" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="12"/>
+      <c r="E19" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E20" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="12"/>
+      <c r="C21" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="E21" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="12"/>
+      <c r="B22" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C22" t="s">
+        <v>339</v>
+      </c>
+      <c r="E22" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="12"/>
+      <c r="B23" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C23" t="s">
+        <v>350</v>
+      </c>
+      <c r="E23" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="12"/>
+      <c r="B24" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="12"/>
+      <c r="B25" s="31" t="s">
+        <v>351</v>
+      </c>
+      <c r="C25" t="s">
+        <v>352</v>
+      </c>
+      <c r="E25" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="12"/>
+      <c r="B26" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" t="s">
+        <v>221</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E26" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="12"/>
+      <c r="B27" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" t="s">
+        <v>216</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E27" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="12"/>
+      <c r="B28" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C28" t="s">
+        <v>227</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E28" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="12"/>
+      <c r="B29" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" t="s">
+        <v>347</v>
+      </c>
+      <c r="E29" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="12"/>
+      <c r="B30" s="10"/>
+      <c r="E30" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="12"/>
+      <c r="B31" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="C31" t="s">
+        <v>346</v>
+      </c>
+      <c r="E31" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="12"/>
+      <c r="E32" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="12"/>
+      <c r="B33" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C33" t="s">
+        <v>344</v>
+      </c>
+      <c r="E33" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="12"/>
+      <c r="E34" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="12"/>
+      <c r="B35" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C35" t="s">
+        <v>345</v>
+      </c>
+      <c r="E35" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="12"/>
+      <c r="E36" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="12"/>
+      <c r="B37" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" t="s">
+        <v>195</v>
+      </c>
+      <c r="E37" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="27" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="12"/>
+      <c r="C38" t="s">
+        <v>353</v>
+      </c>
+      <c r="E38" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="12"/>
+      <c r="C39" t="s">
+        <v>198</v>
+      </c>
+      <c r="E39" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="12"/>
+      <c r="C40" t="s">
+        <v>200</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E40" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="12"/>
+      <c r="E41" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="12"/>
+      <c r="B42" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E42" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="12"/>
+      <c r="E43" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="12"/>
+      <c r="E44" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="12"/>
+      <c r="E45" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="12"/>
+      <c r="B46" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" t="s">
+        <v>210</v>
+      </c>
+      <c r="E46" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" s="12"/>
+      <c r="C47" t="s">
+        <v>211</v>
+      </c>
+      <c r="E47" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="12"/>
+      <c r="E48" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="12"/>
+      <c r="E49" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="12"/>
+      <c r="B50" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="E50" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="12"/>
+      <c r="E51" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" s="12"/>
+      <c r="E52" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53" s="12"/>
+      <c r="E53" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54" s="12"/>
+      <c r="B54" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C54" t="s">
+        <v>309</v>
+      </c>
+      <c r="E54" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55" s="12"/>
+      <c r="C55" t="s">
+        <v>348</v>
+      </c>
+      <c r="E55" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56" s="12"/>
+      <c r="E56" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" s="12"/>
+      <c r="B57" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C57" t="s">
+        <v>272</v>
+      </c>
+      <c r="E57" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A58" s="12"/>
+      <c r="C58" t="s">
+        <v>273</v>
+      </c>
+      <c r="E58" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A59" s="12"/>
+      <c r="C59" t="s">
+        <v>274</v>
+      </c>
+      <c r="E59" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60" s="12"/>
+      <c r="C60" t="s">
+        <v>275</v>
+      </c>
+      <c r="E60" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A61" s="12"/>
+      <c r="C61" t="s">
+        <v>276</v>
+      </c>
+      <c r="E61" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A62" s="12"/>
+      <c r="C62" t="s">
+        <v>277</v>
+      </c>
+      <c r="E62" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A63" s="12"/>
+      <c r="C63" t="s">
+        <v>278</v>
+      </c>
+      <c r="E63" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A64" s="12"/>
+      <c r="C64" t="s">
+        <v>279</v>
+      </c>
+      <c r="E64" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65" s="12"/>
+      <c r="C65" t="s">
+        <v>280</v>
+      </c>
+      <c r="E65" s="25"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66" s="12"/>
+      <c r="E66" s="25"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A67" s="12"/>
+      <c r="E67" s="25"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A68" s="12"/>
+      <c r="E68" s="25"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A69" s="12"/>
+      <c r="E69" s="25"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" s="12"/>
+      <c r="E70" s="25"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71" s="12"/>
+      <c r="E71" s="25"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A72" s="12"/>
+      <c r="E72" s="25"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A73" s="12"/>
+      <c r="E73" s="25"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A74" s="12"/>
+      <c r="E74" s="25"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A75" s="12"/>
+      <c r="E75" s="25"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A76" s="12"/>
+      <c r="E76" s="25"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" s="12"/>
+      <c r="E77" s="25"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A78" s="12"/>
+      <c r="E78" s="25"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A79" s="12"/>
+      <c r="E79" s="25"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A80" s="12"/>
+      <c r="E80" s="25"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A81" s="12"/>
+      <c r="E81" s="25"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G14" r:id="rId1" xr:uid="{82184F06-7443-4019-9CE1-A7ACCF4AFC47}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{B0C4C303-D546-4A05-89EA-6866E2BA24BF}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{DDA2F16C-277F-4D1F-B1B2-DEAAFF1415D1}"/>
+    <hyperlink ref="G37" r:id="rId4" xr:uid="{8C86CF92-79DE-4F42-9876-0397DB56A676}"/>
+    <hyperlink ref="G40" r:id="rId5" xr:uid="{D2623325-AE7E-46B9-84B0-151DE0C14B6E}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{6FCDD72A-7D9C-4F75-9286-1A7D495CD31B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2A7F92-8CC6-47B6-A5ED-C83406DF1ECE}">
+  <dimension ref="A1:G79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.796875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="61.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.265625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="12"/>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="12"/>
+      <c r="B3" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="E4" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="12"/>
+      <c r="B5" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E5" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="12"/>
+      <c r="B6" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="12"/>
+      <c r="B7" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="12"/>
+      <c r="B8" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="E8" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="12"/>
+      <c r="B9" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="12"/>
+      <c r="B10" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="12"/>
+      <c r="B11" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="12"/>
+      <c r="B12" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="E12" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="12"/>
+      <c r="B13" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" t="s">
+        <v>293</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="12"/>
+      <c r="C15" t="s">
+        <v>294</v>
+      </c>
+      <c r="E15" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="12"/>
+      <c r="C16" t="s">
+        <v>295</v>
+      </c>
+      <c r="E16" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" t="s">
+        <v>296</v>
+      </c>
+      <c r="E17" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="12"/>
+      <c r="B18" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="12"/>
+      <c r="C19" t="s">
+        <v>297</v>
+      </c>
+      <c r="E19" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E20" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="12"/>
+      <c r="C21" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="12"/>
+      <c r="C22" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="12"/>
+      <c r="B23" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="E23" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="12"/>
+      <c r="B24" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E24" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="12"/>
+      <c r="B25" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="E25" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="12"/>
+      <c r="B26" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="E26" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="12"/>
+      <c r="B27" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C27" t="s">
+        <v>301</v>
+      </c>
+      <c r="E27" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="12"/>
+      <c r="B28" s="10"/>
+      <c r="E28" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="12"/>
+      <c r="B29" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="C29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="12"/>
+      <c r="E30" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="12"/>
+      <c r="B31" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="C31" t="s">
+        <v>305</v>
+      </c>
+      <c r="E31" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="12"/>
+      <c r="E32" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="12"/>
+      <c r="B33" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C33" t="s">
+        <v>193</v>
+      </c>
+      <c r="E33" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="12"/>
+      <c r="E34" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="12"/>
+      <c r="B35" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E35" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="27" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="12"/>
+      <c r="C36" t="s">
+        <v>196</v>
+      </c>
+      <c r="E36" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="12"/>
+      <c r="C37" t="s">
+        <v>198</v>
+      </c>
+      <c r="E37" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="12"/>
+      <c r="C38" t="s">
+        <v>200</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E38" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="12"/>
+      <c r="E39" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="12"/>
+      <c r="B40" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" t="s">
+        <v>307</v>
+      </c>
+      <c r="E40" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="12"/>
+      <c r="C41" t="s">
+        <v>206</v>
+      </c>
+      <c r="E41" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="12"/>
+      <c r="C42" t="s">
+        <v>207</v>
+      </c>
+      <c r="E42" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="12"/>
+      <c r="E43" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="12"/>
+      <c r="B44" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C44" t="s">
+        <v>210</v>
+      </c>
+      <c r="E44" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="12"/>
+      <c r="C45" t="s">
+        <v>211</v>
+      </c>
+      <c r="E45" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="12"/>
+      <c r="E46" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" s="12"/>
+      <c r="E47" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="12"/>
+      <c r="B48" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="E48" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="12"/>
+      <c r="E49" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="12"/>
+      <c r="E50" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="12"/>
+      <c r="E51" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" s="12"/>
+      <c r="B52" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C52" t="s">
+        <v>309</v>
+      </c>
+      <c r="E52" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53" s="12"/>
+      <c r="E53" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54" s="12"/>
+      <c r="E54" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55" s="12"/>
+      <c r="B55" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C55" t="s">
+        <v>272</v>
+      </c>
+      <c r="E55" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56" s="12"/>
+      <c r="C56" t="s">
+        <v>273</v>
+      </c>
+      <c r="E56" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" s="12"/>
+      <c r="C57" t="s">
+        <v>274</v>
+      </c>
+      <c r="E57" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A58" s="12"/>
+      <c r="C58" t="s">
+        <v>275</v>
+      </c>
+      <c r="E58" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A59" s="12"/>
+      <c r="C59" t="s">
+        <v>276</v>
+      </c>
+      <c r="E59" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60" s="12"/>
+      <c r="C60" t="s">
+        <v>277</v>
+      </c>
+      <c r="E60" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A61" s="12"/>
+      <c r="C61" t="s">
+        <v>278</v>
+      </c>
+      <c r="E61" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A62" s="12"/>
+      <c r="C62" t="s">
+        <v>279</v>
+      </c>
+      <c r="E62" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A63" s="12"/>
+      <c r="C63" t="s">
+        <v>280</v>
+      </c>
+      <c r="E63" s="25"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A64" s="12"/>
+      <c r="E64" s="25"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65" s="12"/>
+      <c r="E65" s="25"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66" s="12"/>
+      <c r="E66" s="25"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A67" s="12"/>
+      <c r="E67" s="25"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A68" s="12"/>
+      <c r="E68" s="25"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A69" s="12"/>
+      <c r="E69" s="25"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" s="12"/>
+      <c r="E70" s="25"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71" s="12"/>
+      <c r="E71" s="25"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A72" s="12"/>
+      <c r="E72" s="25"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A73" s="12"/>
+      <c r="E73" s="25"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A74" s="12"/>
+      <c r="E74" s="25"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A75" s="12"/>
+      <c r="E75" s="25"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A76" s="12"/>
+      <c r="E76" s="25"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" s="12"/>
+      <c r="E77" s="25"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A78" s="12"/>
+      <c r="E78" s="25"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A79" s="12"/>
+      <c r="E79" s="25"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G14" r:id="rId1" xr:uid="{448C13F9-1AD5-4CBD-85FD-80A7C9E098E6}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{5F02D63E-1CBB-4855-B27A-D5B491F1376B}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{BFC786C2-C718-49EB-9C2D-84B62A6B4A96}"/>
+    <hyperlink ref="G35" r:id="rId4" xr:uid="{4A92A8CF-A3DC-4E70-94E5-467E5931157A}"/>
+    <hyperlink ref="G38" r:id="rId5" xr:uid="{820F4BAE-BF6F-4095-9448-B468AAEA9A4A}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{9871AACA-4C84-478E-B5EF-461D982B1F6B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B6397E-9ED3-41BB-8232-94529F745EB9}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="13.06640625" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>1.8</v>
+      </c>
+      <c r="E5">
+        <f>C5/D5</f>
+        <v>8.8888888888888893</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>321</v>
+      </c>
+      <c r="D9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>326</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1.8</v>
+      </c>
+      <c r="E10">
+        <f>C10/D10</f>
+        <v>7.7777777777777777</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" t="s">
+        <v>328</v>
+      </c>
+      <c r="C11">
+        <f>D11*E11</f>
+        <v>46.74</v>
+      </c>
+      <c r="D11">
+        <v>3.8</v>
+      </c>
+      <c r="E11">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>329</v>
+      </c>
+      <c r="C12">
+        <f>D12*E12</f>
+        <v>186.2</v>
+      </c>
+      <c r="D12">
+        <v>3.8</v>
+      </c>
+      <c r="E12">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>330</v>
+      </c>
+      <c r="C13">
+        <f>D13*E13</f>
+        <v>224.2</v>
+      </c>
+      <c r="D13">
+        <v>3.8</v>
+      </c>
+      <c r="E13">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8271526E-A0E8-4F25-B4A3-0A7E74FB5546}">
   <dimension ref="B2:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3645,7 +5565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E0CDA7-FFA5-4B65-AC33-99D61553F876}">
   <dimension ref="A20:Y162"/>
   <sheetViews>
@@ -4174,7 +6094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBA4D58-95DE-4AC6-A317-818729DB4475}">
   <dimension ref="C31"/>
   <sheetViews>

</xml_diff>